<commit_message>
♻️ refactor: eliminate duplication between hardcoded and Excel prompts
**Problem**: Significant overlap between hardcoded prompt in configurator
and Excel Prompts sheet caused maintenance burden and token waste.

**Solution**: Make hardcoded prompt primary, Excel supplementary.

**Changes**:
- Remove 3 prompts with workflow overlap (feature_freeze_prep,
  code_freeze_prep, release_status_check)
- Keep 2 cross-cutting prompts (risk_identification, team_coordination)
- Refactor system_prompt to focus on example questions from test scenarios
- Reduce total prompts from 6 → 3 (50% reduction)
- Reduce system_prompt chars from 1,047 → 756 (28% reduction)

**Benefits**:
- Single source of truth (hardcoded prompt = authoritative)
- No duplication with workflows
- Token efficiency (faster workbook loading)
- Clear separation: code=framework, Excel=examples+cross-cutting
</commit_message>
<xml_diff>
--- a/RHDH_Release_Manager_Reference.xlsx
+++ b/RHDH_Release_Manager_Reference.xlsx
@@ -31,7 +31,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -52,6 +52,9 @@
     <font>
       <name val="Calibri"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -120,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
@@ -156,6 +159,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2203,7 +2209,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2212,205 +2218,111 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="100" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="40" customWidth="1" min="4" max="4"/>
+    <col width="80" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="13" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="13" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="13" t="inlineStr">
         <is>
           <t>prompt_type</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="13" t="inlineStr">
         <is>
           <t>context</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="13" t="inlineStr">
         <is>
           <t>prompt_content</t>
         </is>
       </c>
     </row>
     <row r="2" ht="150" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>system_prompt</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Core system prompt for Release Manager agent</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Core system prompt with example questions</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>system</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Always active - defines agent identity and core capabilities</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>You are the Release Manager for Red Hat Developer Hub (RHDH). Your primary responsibilities are:
-1. Track release progress across Y-stream and Z-stream releases
-2. Provide data-driven insights based on Jira queries and document analysis
-3. Identify risks and blockers proactively
-4. Coordinate information across Engineering, QE, Documentation, and Product Management
-5. Generate release status updates for meetings and stakeholders
-Always prioritize: Accuracy, traceability (provide links), and actionable recommendations.
-Available Tools:
-- Jira tools for querying issues, statistics, and team breakdowns
-- Google Drive tools for reading documents and spreadsheets
-- Release Manager toolkit for queries, templates, and workflows
-General Guidance:
-- Use get_issues_by_team() for team counts (never manual counting)
-- Use get_issues_stats() for quick statistics
-- Always include Jira search links for traceability
-- Format Slack announcements in Markdown for copy-paste delivery
-- Recognize release versions as x.y.z (stream.major.maintenance)</t>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Always active - agent identity and capabilities</t>
+        </is>
+      </c>
+      <c r="E2" s="12" t="inlineStr">
+        <is>
+          <t>You are the Release Manager for Red Hat Developer Hub (RHDH).
+**Core Capabilities:**
+- Query workbook for JQL templates, Slack templates, and workflows
+- Execute Jira queries for release tracking
+- Access Google Drive documents (team data, release schedules)
+- Generate Slack announcements following templates
+**Example Questions You Can Answer:**
+- "What Jira queries are available?"
+- "Show me the Feature Freeze Update template"
+- "How many issues are open in fixVersion 1.9.0?"
+- "Are there any blocker bugs in the current release?"
+- "What are the key dates for active releases?"
+- "List all active RHDH teams with their leads"
+- "Create a code freeze announcement for release 1.9.0"
+- "Break down open issues by team for release 1.9.0"
+- "What are the top 3 risks for releasing version 1.9.0 on time?"
+**Key Principles:**
+- Always use get_issues_by_team() for team counts (never manual counting)
+- Include Jira search links for traceability
+- Format Slack announcements in Markdown code blocks for copy-paste
+- Prioritize accuracy and data-driven insights</t>
         </is>
       </c>
     </row>
     <row r="3" ht="150" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>feature_freeze_prep</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Guidance for preparing Feature Freeze announcement</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>risk_identification</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>How to identify and communicate release risks</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>situational</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Use when user asks to prepare for Feature Freeze</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>When preparing Feature Freeze announcements:
-1. Verify freeze date from release issue using get_issue(RHDHPLAN-XXX)
-2. Gather team issue counts using get_issues_by_team(release_version, team_ids)
-3. Identify outstanding release notes using appropriate JQL query
-4. Check for blockers or risks in issue status
-5. Use Slack template with all placeholders filled
-6. Return in code block (triple backticks) for easy copy-paste into Slack
-7. Use Markdown syntax: [text](url) for links, *bold* for emphasis</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="150" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>code_freeze_prep</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Guidance for preparing Code Freeze announcement</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>situational</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Use when user asks to prepare for Code Freeze</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>When preparing Code Freeze announcements:
-1. Verify code freeze date from release issue using get_issue(RHDHPLAN-XXX)
-2. Gather team issue counts using get_issues_by_team() with code freeze query override if needed
-3. Identify feature subtasks, outstanding release notes
-4. Check for blocker bugs and CVEs
-5. Use Slack template with all placeholders filled
-6. Return in code block (triple backticks) for easy copy-paste
-7. Use Markdown syntax for links and formatting</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="150" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>release_status_check</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>How to provide comprehensive release status</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>situational</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Use when user asks for release status or progress</t>
-        </is>
-      </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>For release status:
-1. Query open issues by type using get_issues_stats()
-2. Identify blockers and CVEs using appropriate JQL queries
-3. Check epic status (epics not in Dev Complete or Release Pending)
-4. Review outstanding release notes
-5. Provide completion percentage based on closed vs total issues
-6. Highlight risks: blocker bugs near freeze, high open counts, missing release notes
-7. Include actionable recommendations for each risk identified</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="150" customHeight="1">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>risk_identification</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>How to identify and communicate release risks</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>situational</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Use when analyzing release health or identifying problems</t>
         </is>
       </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>Risk indicators:
+      <c r="E3" s="12" t="inlineStr">
+        <is>
+          <t>Risk indicators to check:
 1. Blocker bugs near freeze dates - query with priority=blocker filter
 2. High open issue count per team - use get_issues_by_team() to identify overloaded teams
 3. Missing release notes - query issues with empty Release Note Type field
@@ -2424,28 +2336,28 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="150" customHeight="1">
-      <c r="A7" s="2" t="inlineStr">
+    <row r="4" ht="150" customHeight="1">
+      <c r="A4" t="inlineStr">
         <is>
           <t>team_coordination</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>How to coordinate information across teams</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>situational</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Use when generating team-specific updates or breakdowns</t>
         </is>
       </c>
-      <c r="E7" s="3" t="inlineStr">
+      <c r="E4" s="12" t="inlineStr">
         <is>
           <t>For team coordination:
 1. Use get_issues_by_team(release_version, team_ids) for accurate counts (never manual counting!)
@@ -2458,6 +2370,9 @@
         </is>
       </c>
     </row>
+    <row r="5" ht="150" customHeight="1"/>
+    <row r="6" ht="150" customHeight="1"/>
+    <row r="7" ht="150" customHeight="1"/>
   </sheetData>
   <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="0" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="0"/>
   <autoFilter ref="A1:E7"/>

</xml_diff>

<commit_message>
♻️ refactor: add optional trigger phrases support to Release Manager
- Add `trigger_phrases` column support to Jira Queries, Slack Templates, and Actions & Workflows sheets
- Toolkit methods now return 3-tuples (name, description, triggers) instead of 2-tuples
- Add `has_trigger_phrases()` method to detect if sheet has trigger data
- Add `_build_resource_table()` helper to conditionally show Triggers column in system prompt
- Backward compatible: sheets without trigger_phrases column work as before (only show Name | Description)
- Update Excel reference workbook and CSV exports with trigger_phrases examples
- Update AGENTS.md with comprehensive trigger phrases documentation

This enables dynamic pattern matching from workbook data without hardcoding patterns in code.
</commit_message>
<xml_diff>
--- a/RHDH_Release_Manager_Reference.xlsx
+++ b/RHDH_Release_Manager_Reference.xlsx
@@ -530,7 +530,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -562,6 +562,11 @@
           <t>description</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NOTES</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="12" t="inlineStr">
@@ -588,7 +593,7 @@
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>1Dv1JWsQe3Ew82WLFQNhyAwqsn9oEkh2MjoKyHXPuJkk</t>
+          <t>1vQXfvID72qwqvLb17eyGOvnZXrZG7NBzTGv6RP9wvyM</t>
         </is>
       </c>
       <c r="C3" s="12" t="inlineStr">
@@ -611,6 +616,11 @@
       <c r="C4" s="12" t="inlineStr">
         <is>
           <t>Google Drive file ID for Release Schedule spreadsheet (used in future release dates workflow)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>the agent currently is only capable of fetch the first sheet</t>
         </is>
       </c>
     </row>
@@ -2275,27 +2285,21 @@
       </c>
       <c r="E2" s="12" t="inlineStr">
         <is>
-          <t>You are the Release Manager for Red Hat Developer Hub (RHDH).
-**Core Capabilities:**
-- Query workbook for JQL templates, Slack templates, and workflows
-- Execute Jira queries for release tracking
-- Access Google Drive documents (team data, release schedules)
-- Generate Slack announcements following templates
-**Example Questions You Can Answer:**
+          <t>**Example Questions You Can Answer:**
 - "What Jira queries are available?"
 - "Show me the Feature Freeze Update template"
 - "How many issues are open in fixVersion 1.9.0?"
-- "Are there any blocker bugs in the current release?"
-- "What are the key dates for active releases?"
-- "List all active RHDH teams with their leads"
-- "Create a code freeze announcement for release 1.9.0"
-- "Break down open issues by team for release 1.9.0"
-- "What are the top 3 risks for releasing version 1.9.0 on time?"
+- "What workflows are available?"
+- "Get the team breakdown for the current sprint"
+- "List all blocker bugs"
+- "Show the Code Freeze announcement template"
+- "What's the JQL for listing release blockers?"
 **Key Principles:**
 - Always use get_issues_by_team() for team counts (never manual counting)
 - Include Jira search links for traceability
-- Format Slack announcements in Markdown code blocks for copy-paste
-- Prioritize accuracy and data-driven insights</t>
+- Prioritize accuracy and data-driven insights
+**Slack Template handling:**
+- **ALWAYS wrap Slack messages in code blocks** using triple backticks (```slack) for easy copy-paste and tell the user that they can copy-paste this into slack</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2430,6 +2434,11 @@
           <t>notes</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>trigger_phrases</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -2462,6 +2471,11 @@
           <t>Returns release tracking issues with key dates in description</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>"active release" / "release features" / "current release" / "active features"</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -2494,6 +2508,11 @@
           <t>Base query for all open issues in a release</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>"open issues" / "unresolved issues" / "active issues" / "issues for version"</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -2526,6 +2545,11 @@
           <t>Use with issue types: Feature, Epic, Story, Task, Sub-task, Bug, Vulnerability, Weakness</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>"issues by type" / "type breakdown" / "bugs vs stories" / "issue type filter"</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -2558,6 +2582,11 @@
           <t>Identifies EPICs that need attention before release</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>"open epics" / "active epics" / "engineering epics" / "epics in progress"</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
@@ -2590,6 +2619,11 @@
           <t>Critical for security tracking before release</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>"CVEs" / "vulnerabilities" / "security issues" / "security bugs" / "weaknesses"</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -2622,6 +2656,11 @@
           <t>Features that need demo preparation</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>"demo features" / "features for demo" / "demonstration features"</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
@@ -2654,6 +2693,11 @@
           <t>Tracks feature verification and demo creation tasks</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>"feature subtasks" / "acceptance criteria" / "feature tasks"</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -2686,6 +2730,11 @@
           <t>Features ready for Test Day validation</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>"test day" / "test day features" / "features to test"</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
@@ -2718,6 +2767,11 @@
           <t>Tracks scope changes to release</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>"new features" / "recently added" / "features added" / "new to release"</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
@@ -2750,6 +2804,11 @@
           <t>Critical for documentation - must be filled before release</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>"missing release notes" / "release notes needed" / "incomplete release notes"</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
@@ -2782,6 +2841,11 @@
           <t>Excludes infrastructure/ops components and bugs. Use for Feature Freeze announcements.</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>"feature freeze issues" / "outstanding features" / "feature work remaining"</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
@@ -2812,6 +2876,11 @@
       <c r="F13" s="2" t="inlineStr">
         <is>
           <t>All open work. Use for Code Freeze announcements.</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>"code freeze issues" / "outstanding code" / "remaining work" / "open at code freeze"</t>
         </is>
       </c>
     </row>
@@ -2829,7 +2898,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2877,6 +2946,11 @@
           <t>instructions</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>trigger_phrases</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
@@ -2918,6 +2992,11 @@
 5. Include source Jira link for traceability</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>"release dates" / "key dates" / "freeze dates" / "release schedule" / "milestone dates" / "critical dates"</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -2956,6 +3035,11 @@
 2. Extract critical dates for future releases
 3. Format as table with release version and five dates
 4. Include spreadsheet link as source</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>"future releases" / "upcoming releases" / "future schedule" / "release roadmap" / "planned releases"</t>
         </is>
       </c>
     </row>
@@ -2999,6 +3083,11 @@
 5. Include total count across all types</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>"release status" / "active releases" / "release health" / "open issues by release" / "release overview"</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -3040,6 +3129,11 @@
 5. Include spreadsheet link</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>"team list" / "teams and leads" / "team contacts" / "team leads" / "team directory"</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -3080,6 +3174,11 @@
 4. Apply Summary format with total count and Jira link</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>"team breakdown" / "issues by team" / "team workload" / "team counts" / "team assignments"</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
@@ -3120,6 +3219,11 @@
 4. Apply Detailed format with status, priority, assignee</t>
         </is>
       </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>"blocker bugs" / "blockers" / "critical issues" / "blocking issues" / "high priority bugs"</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
@@ -3159,6 +3263,11 @@
 3. Apply Summary format with total and link</t>
         </is>
       </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>"open epics" / "engineering epics" / "active epics" / "epic list" / "epic status"</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -3198,6 +3307,11 @@
 3. Apply Detailed format with severity and status</t>
         </is>
       </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>"CVEs" / "vulnerabilities" / "security issues" / "security bugs" / "list cves"</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="inlineStr">
@@ -3235,6 +3349,11 @@
           <t>1. Execute 'Jira list of release notes' query
 2. Use get_issues_stats() for count
 3. Apply Summary format with total and Jira link</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>"missing release notes" / "release notes needed" / "incomplete release notes" / "release note gaps"</t>
         </is>
       </c>
     </row>
@@ -3279,6 +3398,11 @@
 6. Return in code block (triple backticks) for copy-paste</t>
         </is>
       </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>"feature freeze update" / "feature freeze status" / "update on feature freeze"</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="5" t="inlineStr">
@@ -3318,6 +3442,11 @@
 3. Get outstanding release notes count
 4. Fill Slack template with counts and links
 5. Return in code block for copy-paste</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>"feature freeze announcement" / "announce feature freeze" / "feature freeze milestone"</t>
         </is>
       </c>
     </row>
@@ -3363,6 +3492,11 @@
 7. Return in code block</t>
         </is>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>"code freeze update" / "code freeze status" / "update on code freeze"</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="inlineStr">
@@ -3403,6 +3537,11 @@
 4. Retrieve total open issues count
 5. Fill Slack template with counts and links
 6. Return in code block</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>"code freeze announcement" / "announce code freeze" / "code freeze milestone"</t>
         </is>
       </c>
     </row>
@@ -3420,7 +3559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3458,6 +3597,11 @@
           <t>template_content</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>trigger_phrases</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="300" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
@@ -3493,6 +3637,11 @@
 (repeat for each active engineering team)
 There are [{{OUTSTANDING_RELEASE_NOTES_ISSUE_COUNT}}]({{JIRA_LINK}}) oustanding Release Notes. Please review and update Features and bugs.
 cc @rhdh-release</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>"feature freeze update" / "feature freeze status" / "feature freeze progress"</t>
         </is>
       </c>
     </row>
@@ -3535,6 +3684,11 @@
 cc @rhdh-release</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>"feature freeze announcement" / "announce feature freeze" / "feature freeze reached"</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="300" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
@@ -3572,6 +3726,11 @@
 :two: There are [{{OUTSTANDING_RELEASE_NOTES_ISSUE_COUNT}}]({{JIRA_LINK}}) oustanding Release Notes. Please review and update Features and bugs.
 :three: [{{FEATURE_SUBTASK_ISSUE_COUNT}}]({{JIRA_LINK}}) Feature Subtasks outstanding to verifying Features Acceptance Criteria and creating Feature Demos if needed.
 cc @rhdh-release</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>"code freeze update" / "code freeze status" / "code freeze progress"</t>
         </is>
       </c>
     </row>
@@ -3615,6 +3774,11 @@
 @rhdh-release</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>"code freeze announcement" / "announce code freeze" / "code freeze reached"</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="0" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="0"/>

</xml_diff>